<commit_message>
Updated calculations and added project report
</commit_message>
<xml_diff>
--- a/Specifications/calculations.xlsx
+++ b/Specifications/calculations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\3 My Creations\SPARC\Tesla Coil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\Tesla-Coil\Specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -522,7 +522,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D23"/>
+      <selection activeCell="D23" sqref="A1:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,7 +554,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="4">
-        <v>12000</v>
+        <v>7530</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -576,7 +576,7 @@
         <v>19</v>
       </c>
       <c r="C4">
-        <v>420</v>
+        <v>263.55</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>

</xml_diff>